<commit_message>
Added code for positioning the names based on the length of the names, created multiple pdf files and also merged the pdf files generated and also n added  the code for deleting the files generated
</commit_message>
<xml_diff>
--- a/Certname.xlsx
+++ b/Certname.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MO_WIZZ\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MO_WIZZ\Documents\Python_Project\Certificate_creator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C2926E-7736-4995-BD6C-62049C1273F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5CA7D79-E756-47A9-8DD6-D420983CF15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="6" activeTab="7" xr2:uid="{10A4AAB8-44EF-4F44-91F8-6422F325109A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="6" activeTab="6" xr2:uid="{10A4AAB8-44EF-4F44-91F8-6422F325109A}"/>
   </bookViews>
   <sheets>
     <sheet name="SHORTLIST" sheetId="1" state="hidden" r:id="rId1"/>
@@ -289,7 +289,7 @@
     <author>HP 820 G4</author>
   </authors>
   <commentList>
-    <comment ref="D19" authorId="0" shapeId="0" xr:uid="{DC578526-E66F-4966-A748-EF5AAD4526B8}">
+    <comment ref="E19" authorId="0" shapeId="0" xr:uid="{DC578526-E66F-4966-A748-EF5AAD4526B8}">
       <text>
         <r>
           <rPr>
@@ -352,7 +352,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1722" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1722" uniqueCount="323">
   <si>
     <t>S/N</t>
   </si>
@@ -1313,7 +1313,16 @@
     <t>AKINSOLA FADUNSIN</t>
   </si>
   <si>
+    <t>CERTNAME2</t>
+  </si>
+  <si>
     <t>CERTNAME</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>PHONE</t>
   </si>
 </sst>
 </file>
@@ -2031,7 +2040,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -10411,22 +10420,22 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E91123C-D9E1-4813-8EC4-9F50B5278696}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.28515625" style="134" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="53.140625" customWidth="1"/>
+    <col min="3" max="3" width="42.140625" customWidth="1"/>
+    <col min="4" max="4" width="41.42578125" customWidth="1"/>
+    <col min="5" max="5" width="33.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="145" customFormat="1" ht="15.75" thickBot="1">
+    <row r="1" spans="1:5" s="145" customFormat="1" ht="15.75" thickBot="1">
       <c r="A1" s="157" t="s">
         <v>0</v>
       </c>
@@ -10434,16 +10443,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="146" t="s">
-        <v>261</v>
+        <v>321</v>
       </c>
       <c r="D1" s="146" t="s">
-        <v>294</v>
-      </c>
-      <c r="F1" s="185" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="162" customFormat="1" ht="19.899999999999999" customHeight="1">
+        <v>320</v>
+      </c>
+      <c r="E1" s="146" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="162" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A2" s="159">
         <v>1</v>
       </c>
@@ -10453,15 +10462,15 @@
       <c r="C2" s="160" t="s">
         <v>147</v>
       </c>
-      <c r="D2" s="161" t="s">
+      <c r="D2" s="184" t="str">
+        <f t="shared" ref="D2:D27" si="0">PROPER(B2)</f>
+        <v>Oluwamese Ilesanmi Williams</v>
+      </c>
+      <c r="E2" s="161" t="s">
         <v>148</v>
       </c>
-      <c r="F2" s="184" t="str">
-        <f>PROPER(B2)</f>
-        <v>Oluwamese Ilesanmi Williams</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="162" customFormat="1" ht="19.899999999999999" customHeight="1">
+    </row>
+    <row r="3" spans="1:5" s="162" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A3" s="163">
         <v>2</v>
       </c>
@@ -10471,15 +10480,15 @@
       <c r="C3" s="164" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="165" t="s">
+      <c r="D3" s="184" t="str">
+        <f t="shared" si="0"/>
+        <v>Adaku Inem</v>
+      </c>
+      <c r="E3" s="165" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="184" t="str">
-        <f t="shared" ref="F3:F27" si="0">PROPER(B3)</f>
-        <v>Adaku Inem</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="162" customFormat="1" ht="30" customHeight="1">
+    </row>
+    <row r="4" spans="1:5" s="162" customFormat="1" ht="30" customHeight="1">
       <c r="A4" s="163">
         <v>3</v>
       </c>
@@ -10489,15 +10498,15 @@
       <c r="C4" s="164" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="165" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="184" t="str">
+      <c r="D4" s="184" t="str">
         <f t="shared" si="0"/>
         <v>Okechukwu Obinna Frank</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" s="162" customFormat="1" ht="24" customHeight="1">
+      <c r="E4" s="165" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="162" customFormat="1" ht="24" customHeight="1">
       <c r="A5" s="163">
         <v>4</v>
       </c>
@@ -10507,16 +10516,16 @@
       <c r="C5" s="167" t="s">
         <v>56</v>
       </c>
-      <c r="D5" s="165" t="s">
-        <v>57</v>
-      </c>
-      <c r="F5" s="184" t="str">
+      <c r="D5" s="184" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">
  Chukwuma Williams Adaigbe</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" s="162" customFormat="1" ht="19.899999999999999" customHeight="1">
+      <c r="E5" s="165" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="162" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A6" s="163">
         <v>5</v>
       </c>
@@ -10526,15 +10535,15 @@
       <c r="C6" s="180" t="s">
         <v>315</v>
       </c>
-      <c r="D6" s="165" t="s">
-        <v>316</v>
-      </c>
-      <c r="F6" s="184" t="str">
+      <c r="D6" s="184" t="str">
         <f t="shared" si="0"/>
         <v>Ajisafe Marvelous</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" s="162" customFormat="1" ht="19.899999999999999" customHeight="1">
+      <c r="E6" s="165" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="162" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A7" s="163">
         <v>6</v>
       </c>
@@ -10544,15 +10553,15 @@
       <c r="C7" s="168" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="165" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="184" t="str">
+      <c r="D7" s="184" t="str">
         <f t="shared" si="0"/>
         <v>Megwatam Chidiebere Timothy</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" s="162" customFormat="1" ht="19.899999999999999" customHeight="1">
+      <c r="E7" s="165" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="162" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A8" s="163">
         <v>7</v>
       </c>
@@ -10562,15 +10571,15 @@
       <c r="C8" s="164" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="165" t="s">
-        <v>75</v>
-      </c>
-      <c r="F8" s="184" t="str">
+      <c r="D8" s="184" t="str">
         <f t="shared" si="0"/>
         <v>Ojini Joshua</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" s="162" customFormat="1" ht="19.899999999999999" customHeight="1">
+      <c r="E8" s="165" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="162" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A9" s="163">
         <v>8</v>
       </c>
@@ -10580,15 +10589,15 @@
       <c r="C9" s="180" t="s">
         <v>111</v>
       </c>
-      <c r="D9" s="165" t="s">
-        <v>112</v>
-      </c>
-      <c r="F9" s="184" t="str">
+      <c r="D9" s="184" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">Okere Emmanuel </v>
       </c>
-    </row>
-    <row r="10" spans="1:6" s="162" customFormat="1">
+      <c r="E9" s="165" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="162" customFormat="1">
       <c r="A10" s="163">
         <v>9</v>
       </c>
@@ -10598,15 +10607,15 @@
       <c r="C10" s="164" t="s">
         <v>141</v>
       </c>
-      <c r="D10" s="169" t="s">
-        <v>142</v>
-      </c>
-      <c r="F10" s="184" t="str">
+      <c r="D10" s="184" t="str">
         <f t="shared" si="0"/>
         <v>Balikis Motunrayo Alli</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" s="162" customFormat="1" ht="15.75" thickBot="1">
+      <c r="E10" s="169" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="162" customFormat="1" ht="15.75" thickBot="1">
       <c r="A11" s="163">
         <v>10</v>
       </c>
@@ -10616,15 +10625,15 @@
       <c r="C11" s="171" t="s">
         <v>231</v>
       </c>
-      <c r="D11" s="172" t="s">
-        <v>254</v>
-      </c>
-      <c r="F11" s="184" t="str">
+      <c r="D11" s="184" t="str">
         <f t="shared" si="0"/>
         <v>Garuba Aishat</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" s="110" customFormat="1">
+      <c r="E11" s="172" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="110" customFormat="1">
       <c r="A12" s="119">
         <v>11</v>
       </c>
@@ -10634,15 +10643,15 @@
       <c r="C12" s="149" t="s">
         <v>236</v>
       </c>
-      <c r="D12" s="150" t="s">
-        <v>237</v>
-      </c>
-      <c r="F12" s="184" t="str">
+      <c r="D12" s="184" t="str">
         <f t="shared" si="0"/>
         <v>Oluwatobi Olajide</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" s="110" customFormat="1">
+      <c r="E12" s="150" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="110" customFormat="1">
       <c r="A13" s="119">
         <v>12</v>
       </c>
@@ -10652,15 +10661,15 @@
       <c r="C13" s="120" t="s">
         <v>209</v>
       </c>
-      <c r="D13" s="121" t="s">
-        <v>210</v>
-      </c>
-      <c r="F13" s="184" t="str">
+      <c r="D13" s="184" t="str">
         <f t="shared" si="0"/>
         <v>Favour Adekogbe</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" s="110" customFormat="1">
+      <c r="E13" s="121" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="110" customFormat="1">
       <c r="A14" s="119">
         <v>13</v>
       </c>
@@ -10670,15 +10679,15 @@
       <c r="C14" s="120" t="s">
         <v>218</v>
       </c>
-      <c r="D14" s="121" t="s">
-        <v>219</v>
-      </c>
-      <c r="F14" s="184" t="str">
+      <c r="D14" s="184" t="str">
         <f t="shared" si="0"/>
         <v>Egberiemu Ovie Daniel</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" s="110" customFormat="1">
+      <c r="E14" s="121" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="110" customFormat="1">
       <c r="A15" s="119">
         <v>14</v>
       </c>
@@ -10688,15 +10697,15 @@
       <c r="C15" s="120" t="s">
         <v>205</v>
       </c>
-      <c r="D15" s="121" t="s">
-        <v>206</v>
-      </c>
-      <c r="F15" s="184" t="str">
+      <c r="D15" s="184" t="str">
         <f t="shared" si="0"/>
         <v>Adekoya Taqwallah Titilope</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" s="110" customFormat="1">
+      <c r="E15" s="121" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="110" customFormat="1">
       <c r="A16" s="119">
         <v>15</v>
       </c>
@@ -10706,15 +10715,15 @@
       <c r="C16" s="120" t="s">
         <v>191</v>
       </c>
-      <c r="D16" s="152" t="s">
-        <v>192</v>
-      </c>
-      <c r="F16" s="184" t="str">
+      <c r="D16" s="184" t="str">
         <f t="shared" si="0"/>
         <v>Joshua Okwueze Osolu</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" s="110" customFormat="1">
+      <c r="E16" s="152" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="110" customFormat="1">
       <c r="A17" s="119">
         <v>16</v>
       </c>
@@ -10724,15 +10733,15 @@
       <c r="C17" s="148" t="s">
         <v>244</v>
       </c>
-      <c r="D17" s="153" t="s">
-        <v>253</v>
-      </c>
-      <c r="F17" s="184" t="str">
+      <c r="D17" s="184" t="str">
         <f t="shared" si="0"/>
         <v>Agbogo John Asu</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" s="110" customFormat="1">
+      <c r="E17" s="153" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="110" customFormat="1">
       <c r="A18" s="119">
         <v>17</v>
       </c>
@@ -10742,15 +10751,15 @@
       <c r="C18" s="148" t="s">
         <v>232</v>
       </c>
-      <c r="D18" s="104" t="s">
-        <v>221</v>
-      </c>
-      <c r="F18" s="184" t="str">
+      <c r="D18" s="184" t="str">
         <f t="shared" si="0"/>
         <v>Jerry Nnamdi Nwaru</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" s="110" customFormat="1" ht="19.899999999999999" customHeight="1">
+      <c r="E18" s="104" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="110" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A19" s="119">
         <v>18</v>
       </c>
@@ -10760,15 +10769,15 @@
       <c r="C19" s="120" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="142" t="s">
-        <v>28</v>
-      </c>
-      <c r="F19" s="184" t="str">
+      <c r="D19" s="184" t="str">
         <f t="shared" si="0"/>
         <v>Tolulope Oyebode</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" s="110" customFormat="1">
+      <c r="E19" s="142" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="110" customFormat="1">
       <c r="A20" s="119">
         <v>19</v>
       </c>
@@ -10778,15 +10787,15 @@
       <c r="C20" s="148" t="s">
         <v>246</v>
       </c>
-      <c r="D20" s="153">
-        <v>7031593733</v>
-      </c>
-      <c r="F20" s="184" t="str">
+      <c r="D20" s="184" t="str">
         <f t="shared" si="0"/>
         <v>Adekunle Tosin Taiwo</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" s="110" customFormat="1">
+      <c r="E20" s="153">
+        <v>7031593733</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="110" customFormat="1">
       <c r="A21" s="119">
         <v>20</v>
       </c>
@@ -10796,15 +10805,15 @@
       <c r="C21" s="120" t="s">
         <v>197</v>
       </c>
-      <c r="D21" s="121" t="s">
-        <v>198</v>
-      </c>
-      <c r="F21" s="184" t="str">
+      <c r="D21" s="184" t="str">
         <f t="shared" si="0"/>
         <v>Onyekachukwu Abike Aribeana</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" s="110" customFormat="1">
+      <c r="E21" s="121" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="110" customFormat="1">
       <c r="A22" s="119">
         <v>21</v>
       </c>
@@ -10814,15 +10823,15 @@
       <c r="C22" s="120" t="s">
         <v>183</v>
       </c>
-      <c r="D22" s="152" t="s">
-        <v>184</v>
-      </c>
-      <c r="F22" s="184" t="str">
+      <c r="D22" s="184" t="str">
         <f t="shared" si="0"/>
         <v>Afolabi Zainab Oluwapelumi</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" s="110" customFormat="1">
+      <c r="E22" s="152" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="110" customFormat="1">
       <c r="A23" s="139">
         <v>22</v>
       </c>
@@ -10832,15 +10841,15 @@
       <c r="C23" s="140" t="s">
         <v>181</v>
       </c>
-      <c r="D23" s="141" t="s">
-        <v>180</v>
-      </c>
-      <c r="F23" s="184" t="str">
+      <c r="D23" s="184" t="str">
         <f t="shared" si="0"/>
         <v>Akintan Oluwamodupe Esther</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" s="144" customFormat="1">
+      <c r="E23" s="141" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" s="144" customFormat="1">
       <c r="A24" s="158">
         <v>23</v>
       </c>
@@ -10850,15 +10859,15 @@
       <c r="C24" s="155" t="s">
         <v>163</v>
       </c>
-      <c r="D24" s="156" t="s">
-        <v>164</v>
-      </c>
-      <c r="F24" s="184" t="str">
+      <c r="D24" s="184" t="str">
         <f t="shared" si="0"/>
         <v>Andrew Omo</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" s="128" customFormat="1">
+      <c r="E24" s="156" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="128" customFormat="1">
       <c r="A25" s="147">
         <v>24</v>
       </c>
@@ -10868,15 +10877,15 @@
       <c r="C25" s="47" t="s">
         <v>295</v>
       </c>
-      <c r="D25" s="136" t="s">
-        <v>176</v>
-      </c>
-      <c r="F25" s="184" t="str">
+      <c r="D25" s="184" t="str">
         <f t="shared" si="0"/>
         <v>Nnamah Ifeoma.</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" s="134" customFormat="1">
+      <c r="E25" s="136" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="134" customFormat="1">
       <c r="A26" s="119">
         <v>25</v>
       </c>
@@ -10886,16 +10895,16 @@
       <c r="C26" s="135" t="s">
         <v>268</v>
       </c>
-      <c r="D26" s="136" t="s">
+      <c r="D26" s="184" t="str">
+        <f t="shared" si="0"/>
+        <v>Doumu Tariere Jessica</v>
+      </c>
+      <c r="E26" s="136" t="s">
         <v>269</v>
       </c>
-      <c r="F26" s="184" t="str">
-        <f>PROPER(B26)</f>
-        <v>Doumu Tariere Jessica</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="F27" s="184" t="str">
+    </row>
+    <row r="27" spans="1:5">
+      <c r="D27" s="184" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -10934,22 +10943,22 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7838A8EE-709E-4277-BDD6-010BE6A4DDA7}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.42578125" customWidth="1"/>
+    <col min="2" max="2" width="46.5703125" customWidth="1"/>
+    <col min="3" max="3" width="43.5703125" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" customWidth="1"/>
+    <col min="5" max="5" width="38.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="19.5" thickBot="1">
+    <row r="1" spans="1:9" ht="19.5" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10959,14 +10968,14 @@
       <c r="C1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="185" t="s">
+        <v>319</v>
+      </c>
+      <c r="E1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="93" customFormat="1" ht="19.899999999999999" customHeight="1">
+    </row>
+    <row r="2" spans="1:9" s="93" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A2" s="94">
         <v>1</v>
       </c>
@@ -10976,15 +10985,15 @@
       <c r="C2" s="95" t="s">
         <v>154</v>
       </c>
-      <c r="D2" s="55" t="s">
+      <c r="D2" s="93" t="str">
+        <f t="shared" ref="D2:D27" si="0">PROPER(B2)</f>
+        <v>Itarin Andrew Babatunde</v>
+      </c>
+      <c r="E2" s="55" t="s">
         <v>155</v>
       </c>
-      <c r="E2" s="93" t="str">
-        <f>PROPER(B2)</f>
-        <v>Itarin Andrew Babatunde</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="93" customFormat="1" ht="19.899999999999999" customHeight="1">
+    </row>
+    <row r="3" spans="1:9" s="93" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A3" s="94">
         <v>2</v>
       </c>
@@ -10994,15 +11003,15 @@
       <c r="C3" s="95" t="s">
         <v>71</v>
       </c>
-      <c r="D3" s="96" t="s">
+      <c r="D3" s="93" t="str">
+        <f t="shared" si="0"/>
+        <v>Agbo Samuel E.</v>
+      </c>
+      <c r="E3" s="96" t="s">
         <v>72</v>
       </c>
-      <c r="E3" s="93" t="str">
-        <f t="shared" ref="E3:E27" si="0">PROPER(B3)</f>
-        <v>Agbo Samuel E.</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="93" customFormat="1" ht="19.899999999999999" customHeight="1">
+    </row>
+    <row r="4" spans="1:9" s="93" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A4" s="94">
         <v>3</v>
       </c>
@@ -11012,15 +11021,15 @@
       <c r="C4" s="95" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="96" t="s">
-        <v>78</v>
-      </c>
-      <c r="E4" s="93" t="str">
+      <c r="D4" s="93" t="str">
         <f t="shared" si="0"/>
         <v>Amina Bintu Muhammed</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" s="93" customFormat="1" ht="19.899999999999999" customHeight="1">
+      <c r="E4" s="96" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="93" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A5" s="94">
         <v>4</v>
       </c>
@@ -11030,15 +11039,15 @@
       <c r="C5" s="95" t="s">
         <v>83</v>
       </c>
-      <c r="D5" s="96" t="s">
-        <v>84</v>
-      </c>
-      <c r="E5" s="93" t="str">
+      <c r="D5" s="93" t="str">
         <f t="shared" si="0"/>
         <v>Joshua Enebeli</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" s="93" customFormat="1" ht="19.899999999999999" customHeight="1">
+      <c r="E5" s="96" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="93" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A6" s="94">
         <v>5</v>
       </c>
@@ -11048,18 +11057,18 @@
       <c r="C6" s="95" t="s">
         <v>114</v>
       </c>
-      <c r="D6" s="55" t="s">
-        <v>115</v>
-      </c>
-      <c r="E6" s="93" t="str">
+      <c r="D6" s="93" t="str">
         <f t="shared" si="0"/>
         <v>Eze Osinachi A</v>
       </c>
-      <c r="F6"/>
+      <c r="E6" s="55" t="s">
+        <v>115</v>
+      </c>
       <c r="G6"/>
       <c r="H6"/>
-    </row>
-    <row r="7" spans="1:8" s="93" customFormat="1" ht="19.899999999999999" customHeight="1">
+      <c r="I6"/>
+    </row>
+    <row r="7" spans="1:9" s="93" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A7" s="94">
         <v>6</v>
       </c>
@@ -11069,18 +11078,18 @@
       <c r="C7" s="95" t="s">
         <v>126</v>
       </c>
-      <c r="D7" s="55" t="s">
-        <v>127</v>
-      </c>
-      <c r="E7" s="93" t="str">
+      <c r="D7" s="93" t="str">
         <f t="shared" si="0"/>
         <v>Daraojimba Andrew Ifesinachi</v>
       </c>
-      <c r="F7"/>
+      <c r="E7" s="55" t="s">
+        <v>127</v>
+      </c>
       <c r="G7"/>
       <c r="H7"/>
-    </row>
-    <row r="8" spans="1:8" s="93" customFormat="1">
+      <c r="I7"/>
+    </row>
+    <row r="8" spans="1:9" s="93" customFormat="1">
       <c r="A8" s="94">
         <v>7</v>
       </c>
@@ -11090,18 +11099,18 @@
       <c r="C8" s="97" t="s">
         <v>252</v>
       </c>
-      <c r="D8" s="98" t="s">
-        <v>255</v>
-      </c>
-      <c r="E8" s="93" t="str">
+      <c r="D8" s="93" t="str">
         <f t="shared" si="0"/>
         <v>Eziora Christian</v>
       </c>
-      <c r="F8"/>
+      <c r="E8" s="98" t="s">
+        <v>255</v>
+      </c>
       <c r="G8"/>
       <c r="H8"/>
-    </row>
-    <row r="9" spans="1:8" s="93" customFormat="1" ht="19.899999999999999" customHeight="1">
+      <c r="I8"/>
+    </row>
+    <row r="9" spans="1:9" s="93" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A9" s="94">
         <v>8</v>
       </c>
@@ -11111,18 +11120,18 @@
       <c r="C9" s="95" t="s">
         <v>99</v>
       </c>
-      <c r="D9" s="55" t="s">
-        <v>100</v>
-      </c>
-      <c r="E9" s="93" t="str">
+      <c r="D9" s="93" t="str">
         <f t="shared" si="0"/>
         <v>Agupusi Isaac Izunna</v>
       </c>
-      <c r="F9"/>
+      <c r="E9" s="55" t="s">
+        <v>100</v>
+      </c>
       <c r="G9"/>
       <c r="H9"/>
-    </row>
-    <row r="10" spans="1:8" s="184" customFormat="1" ht="19.899999999999999" customHeight="1">
+      <c r="I9"/>
+    </row>
+    <row r="10" spans="1:9" s="184" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A10" s="181">
         <v>9</v>
       </c>
@@ -11132,18 +11141,18 @@
       <c r="C10" s="182" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="183" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="93" t="str">
+      <c r="D10" s="93" t="str">
         <f t="shared" si="0"/>
         <v>Balogun Kabiru Olawale</v>
       </c>
-      <c r="F10" s="20"/>
+      <c r="E10" s="183" t="s">
+        <v>9</v>
+      </c>
       <c r="G10" s="20"/>
       <c r="H10" s="20"/>
-    </row>
-    <row r="11" spans="1:8" s="93" customFormat="1">
+      <c r="I10" s="20"/>
+    </row>
+    <row r="11" spans="1:9" s="93" customFormat="1">
       <c r="A11" s="94">
         <v>10</v>
       </c>
@@ -11153,18 +11162,18 @@
       <c r="C11" s="95" t="s">
         <v>203</v>
       </c>
-      <c r="D11" s="55" t="s">
-        <v>204</v>
-      </c>
-      <c r="E11" s="93" t="str">
+      <c r="D11" s="93" t="str">
         <f t="shared" si="0"/>
         <v>Ekene Ike-Okoro Anthony</v>
       </c>
-      <c r="F11"/>
+      <c r="E11" s="55" t="s">
+        <v>204</v>
+      </c>
       <c r="G11"/>
       <c r="H11"/>
-    </row>
-    <row r="12" spans="1:8" s="93" customFormat="1">
+      <c r="I11"/>
+    </row>
+    <row r="12" spans="1:9" s="93" customFormat="1">
       <c r="A12" s="94">
         <v>11</v>
       </c>
@@ -11174,18 +11183,18 @@
       <c r="C12" s="95" t="s">
         <v>212</v>
       </c>
-      <c r="D12" s="55" t="s">
-        <v>213</v>
-      </c>
-      <c r="E12" s="93" t="str">
+      <c r="D12" s="93" t="str">
         <f t="shared" si="0"/>
         <v>Olatunji Gabriel Omogbolahan</v>
       </c>
-      <c r="F12"/>
+      <c r="E12" s="55" t="s">
+        <v>213</v>
+      </c>
       <c r="G12"/>
       <c r="H12"/>
-    </row>
-    <row r="13" spans="1:8" s="93" customFormat="1">
+      <c r="I12"/>
+    </row>
+    <row r="13" spans="1:9" s="93" customFormat="1">
       <c r="A13" s="94">
         <v>12</v>
       </c>
@@ -11195,20 +11204,20 @@
       <c r="C13" s="95" t="s">
         <v>194</v>
       </c>
-      <c r="D13" s="55" t="s">
-        <v>195</v>
-      </c>
-      <c r="E13" s="93" t="str">
+      <c r="D13" s="93" t="str">
         <f t="shared" si="0"/>
         <v>Ikhianosen Omata Ehizokhale</v>
       </c>
-      <c r="F13"/>
+      <c r="E13" s="55" t="s">
+        <v>195</v>
+      </c>
       <c r="G13"/>
-      <c r="H13" t="s">
+      <c r="H13"/>
+      <c r="I13" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="122" customFormat="1">
+    <row r="14" spans="1:9" s="122" customFormat="1">
       <c r="A14" s="94">
         <v>13</v>
       </c>
@@ -11218,18 +11227,18 @@
       <c r="C14" s="120" t="s">
         <v>215</v>
       </c>
-      <c r="D14" s="121" t="s">
-        <v>216</v>
-      </c>
-      <c r="E14" s="93" t="str">
+      <c r="D14" s="93" t="str">
         <f t="shared" si="0"/>
         <v>Opirite Bilaye Tariah</v>
       </c>
-      <c r="F14"/>
+      <c r="E14" s="121" t="s">
+        <v>216</v>
+      </c>
       <c r="G14"/>
       <c r="H14"/>
-    </row>
-    <row r="15" spans="1:8" s="93" customFormat="1">
+      <c r="I14"/>
+    </row>
+    <row r="15" spans="1:9" s="93" customFormat="1">
       <c r="A15" s="94">
         <v>14</v>
       </c>
@@ -11239,15 +11248,15 @@
       <c r="C15" s="95" t="s">
         <v>200</v>
       </c>
-      <c r="D15" s="55" t="s">
-        <v>201</v>
-      </c>
-      <c r="E15" s="93" t="str">
+      <c r="D15" s="93" t="str">
         <f t="shared" si="0"/>
         <v>Ojiruen Idiegbeyaose Christabel</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" s="93" customFormat="1">
+      <c r="E15" s="55" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="93" customFormat="1">
       <c r="A16" s="94">
         <v>15</v>
       </c>
@@ -11257,15 +11266,15 @@
       <c r="C16" s="95" t="s">
         <v>187</v>
       </c>
-      <c r="D16" s="102" t="s">
-        <v>186</v>
-      </c>
-      <c r="E16" s="93" t="str">
+      <c r="D16" s="93" t="str">
         <f t="shared" si="0"/>
         <v>Winifred Onyinyechi Ejioronu</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" s="93" customFormat="1">
+      <c r="E16" s="102" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="93" customFormat="1">
       <c r="A17" s="94">
         <v>16</v>
       </c>
@@ -11275,30 +11284,30 @@
       <c r="C17" s="100" t="s">
         <v>188</v>
       </c>
-      <c r="D17" s="103">
-        <v>8135805107</v>
-      </c>
-      <c r="E17" s="93" t="str">
+      <c r="D17" s="93" t="str">
         <f t="shared" si="0"/>
         <v>Stanley Nwaru Ndubusi</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" s="93" customFormat="1">
+      <c r="E17" s="103">
+        <v>8135805107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="93" customFormat="1">
       <c r="A18" s="94">
         <v>17</v>
       </c>
       <c r="B18" s="104" t="s">
         <v>310</v>
       </c>
-      <c r="D18" s="104" t="s">
-        <v>223</v>
-      </c>
-      <c r="E18" s="93" t="str">
+      <c r="D18" s="93" t="str">
         <f t="shared" si="0"/>
         <v>Lawal  Moruf Ayobami</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" s="93" customFormat="1">
+      <c r="E18" s="104" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="93" customFormat="1">
       <c r="A19" s="94">
         <v>18</v>
       </c>
@@ -11308,15 +11317,15 @@
       <c r="C19" s="100" t="s">
         <v>241</v>
       </c>
-      <c r="D19" s="104" t="s">
-        <v>225</v>
-      </c>
-      <c r="E19" s="93" t="str">
+      <c r="D19" s="93" t="str">
         <f t="shared" si="0"/>
         <v>Toriade Adedeji</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" s="93" customFormat="1">
+      <c r="E19" s="104" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="93" customFormat="1">
       <c r="A20" s="94">
         <v>19</v>
       </c>
@@ -11326,15 +11335,15 @@
       <c r="C20" s="100" t="s">
         <v>242</v>
       </c>
-      <c r="D20" s="104" t="s">
-        <v>317</v>
-      </c>
-      <c r="E20" s="93" t="str">
+      <c r="D20" s="93" t="str">
         <f t="shared" si="0"/>
         <v>Akinsola Fadunsin</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" s="93" customFormat="1" ht="15.75" thickBot="1">
+      <c r="E20" s="104" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="93" customFormat="1" ht="15.75" thickBot="1">
       <c r="A21" s="94">
         <v>20</v>
       </c>
@@ -11344,15 +11353,15 @@
       <c r="C21" s="105" t="s">
         <v>229</v>
       </c>
-      <c r="D21" s="106" t="s">
-        <v>312</v>
-      </c>
-      <c r="E21" s="93" t="str">
+      <c r="D21" s="93" t="str">
         <f t="shared" si="0"/>
         <v>Ogundijo Nimota Adunni</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" s="122" customFormat="1" ht="19.899999999999999" customHeight="1">
+      <c r="E21" s="106" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="122" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A22" s="94">
         <v>21</v>
       </c>
@@ -11362,15 +11371,15 @@
       <c r="C22" s="120" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="142" t="s">
-        <v>35</v>
-      </c>
-      <c r="E22" s="93" t="str">
+      <c r="D22" s="93" t="str">
         <f t="shared" si="0"/>
         <v>Chimaobim Ekere</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" s="134" customFormat="1">
+      <c r="E22" s="142" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="134" customFormat="1">
       <c r="A23" s="94">
         <v>22</v>
       </c>
@@ -11380,15 +11389,15 @@
       <c r="C23" s="174" t="s">
         <v>277</v>
       </c>
-      <c r="D23" s="175" t="s">
-        <v>278</v>
-      </c>
-      <c r="E23" s="93" t="str">
+      <c r="D23" s="93" t="str">
         <f t="shared" si="0"/>
         <v>Akinyele Oluwagbenga</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" s="134" customFormat="1">
+      <c r="E23" s="175" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" s="134" customFormat="1">
       <c r="A24" s="94">
         <v>23</v>
       </c>
@@ -11398,15 +11407,15 @@
       <c r="C24" s="174" t="s">
         <v>281</v>
       </c>
-      <c r="D24" s="175" t="s">
-        <v>282</v>
-      </c>
-      <c r="E24" s="93" t="str">
+      <c r="D24" s="93" t="str">
         <f t="shared" si="0"/>
         <v>Ife-Michael Onofue Victoria</v>
       </c>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="E24" s="175" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" s="94">
         <v>24</v>
       </c>
@@ -11416,16 +11425,16 @@
       <c r="C25" s="177" t="s">
         <v>296</v>
       </c>
-      <c r="D25" s="178" t="s">
-        <v>297</v>
-      </c>
-      <c r="E25" s="93" t="str">
+      <c r="D25" s="93" t="str">
         <f t="shared" si="0"/>
         <v>Adebakin Halimat Ololade</v>
       </c>
-      <c r="H25" s="143"/>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="E25" s="178" t="s">
+        <v>297</v>
+      </c>
+      <c r="I25" s="143"/>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" s="94">
         <v>25</v>
       </c>
@@ -11433,18 +11442,18 @@
         <v>311</v>
       </c>
       <c r="C26" s="179"/>
-      <c r="D26" s="178" t="s">
-        <v>298</v>
-      </c>
-      <c r="E26" s="93" t="str">
+      <c r="D26" s="93" t="str">
         <f t="shared" si="0"/>
         <v>Victory Oliaku</v>
       </c>
-      <c r="H26" s="134"/>
+      <c r="E26" s="178" t="s">
+        <v>298</v>
+      </c>
       <c r="I26" s="134"/>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="E27" s="93" t="str">
+      <c r="J26" s="134"/>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="D27" s="93" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>

</xml_diff>